<commit_message>
tes excel lampiran 2 rks barang penunjukan langsung
</commit_message>
<xml_diff>
--- a/templates/PL-B-Lamp_2.xlsx
+++ b/templates/PL-B-Lamp_2.xlsx
@@ -40,9 +40,6 @@
     <t xml:space="preserve">               PENGADAAN BARANG ..................................................................</t>
   </si>
   <si>
-    <t>PT PLN (PERSERO) .....................</t>
-  </si>
-  <si>
     <t>NOMOR</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t xml:space="preserve">               RKS PENUNJUKAN LANGSUNG</t>
+  </si>
+  <si>
+    <t>PT PLN (PERSERO) KANTOR PUSAT</t>
   </si>
 </sst>
 </file>
@@ -592,30 +592,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -687,6 +663,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1069,7 +1069,7 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="B6" sqref="B6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1089,7 +1089,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="60" t="s">
+      <c r="H1" s="52" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1121,12 +1121,12 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15">
       <c r="B5" s="63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="62"/>
       <c r="D5" s="62"/>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="6" spans="2:8" ht="15">
       <c r="B6" s="63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="62"/>
       <c r="D6" s="62"/>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="7" spans="2:8" ht="15">
       <c r="B7" s="63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="62"/>
       <c r="D7" s="62"/>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="9" spans="2:8" ht="15">
       <c r="B9" s="63" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="C9" s="62"/>
       <c r="D9" s="62"/>
@@ -1198,78 +1198,78 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:8" ht="14.25" thickTop="1" thickBot="1">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17" t="s">
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="53"/>
+      <c r="F12" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18" t="s">
+      <c r="G12" s="55"/>
+      <c r="H12" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20" t="s">
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="57" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="2:8">
-      <c r="B13" s="21" t="s">
+      <c r="C13" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="D13" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="E13" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="G13" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="13.5" thickBot="1">
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="59"/>
+      <c r="H14" s="60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="13.5" thickBot="1">
+      <c r="B15" s="24">
+        <v>1</v>
+      </c>
+      <c r="C15" s="24">
+        <v>2</v>
+      </c>
+      <c r="D15" s="24">
+        <v>3</v>
+      </c>
+      <c r="E15" s="24">
+        <v>4</v>
+      </c>
+      <c r="F15" s="24">
+        <v>5</v>
+      </c>
+      <c r="G15" s="24">
         <v>6</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="13.5" thickBot="1">
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="13.5" thickBot="1">
-      <c r="B15" s="32">
-        <v>1</v>
-      </c>
-      <c r="C15" s="32">
-        <v>2</v>
-      </c>
-      <c r="D15" s="32">
-        <v>3</v>
-      </c>
-      <c r="E15" s="32">
-        <v>4</v>
-      </c>
-      <c r="F15" s="32">
-        <v>5</v>
-      </c>
-      <c r="G15" s="32">
-        <v>6</v>
-      </c>
-      <c r="H15" s="54">
+      <c r="H15" s="46">
         <v>7</v>
       </c>
     </row>
@@ -1644,40 +1644,40 @@
     </row>
     <row r="57" spans="2:8">
       <c r="B57" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="58"/>
+      <c r="G57" s="50"/>
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="2:8" ht="13.5" thickBot="1">
       <c r="B58" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
-      <c r="G58" s="59"/>
+      <c r="G58" s="51"/>
       <c r="H58" s="3"/>
     </row>
     <row r="59" spans="2:8" ht="13.5" thickBot="1">
       <c r="B59" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
-      <c r="G59" s="59"/>
+      <c r="G59" s="51"/>
       <c r="H59" s="3"/>
     </row>
     <row r="60" spans="2:8" ht="13.5" thickBot="1">
       <c r="B60" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
@@ -1687,72 +1687,72 @@
       <c r="H60" s="7"/>
     </row>
     <row r="61" spans="2:8" ht="13.5" thickTop="1">
-      <c r="B61" s="55"/>
-      <c r="C61" s="56"/>
-      <c r="D61" s="56"/>
-      <c r="E61" s="56"/>
-      <c r="F61" s="56"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="56"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="48"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
     </row>
     <row r="62" spans="2:8">
-      <c r="B62" s="57" t="s">
+      <c r="B62" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="49"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="49"/>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="57"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="57"/>
-      <c r="F62" s="57"/>
-      <c r="G62" s="57"/>
-      <c r="H62" s="57"/>
-    </row>
-    <row r="63" spans="2:8">
-      <c r="B63" s="57" t="s">
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C63" s="57"/>
-      <c r="D63" s="57"/>
-      <c r="E63" s="57"/>
-      <c r="F63" s="57"/>
-      <c r="G63" s="57"/>
-      <c r="H63" s="57"/>
-    </row>
-    <row r="64" spans="2:8">
-      <c r="B64" s="57" t="s">
+      <c r="C64" s="49"/>
+      <c r="D64" s="49"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="49"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="B65" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="57"/>
-      <c r="D64" s="57"/>
-      <c r="E64" s="57"/>
-      <c r="F64" s="57"/>
-      <c r="G64" s="57"/>
-      <c r="H64" s="57"/>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="B65" s="57" t="s">
+      <c r="C65" s="49"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="49"/>
+      <c r="F65" s="49"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="49"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="B66" s="47"/>
+      <c r="C66" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C65" s="57"/>
-      <c r="D65" s="57"/>
-      <c r="E65" s="57"/>
-      <c r="F65" s="57"/>
-      <c r="G65" s="57"/>
-      <c r="H65" s="57"/>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="B66" s="55"/>
-      <c r="C66" s="57" t="s">
+      <c r="D66" s="48"/>
+      <c r="E66" s="48"/>
+      <c r="F66" s="48"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="48"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="45" t="s">
         <v>24</v>
-      </c>
-      <c r="D66" s="56"/>
-      <c r="E66" s="56"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="56"/>
-      <c r="H66" s="56"/>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="53" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1914,16 +1914,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:7">
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="17" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="3:7">
-      <c r="G2" s="25"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="3:7" ht="15">
       <c r="C3" s="63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="62"/>
       <c r="E3" s="62"/>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="4" spans="3:7" ht="15">
       <c r="C4" s="63" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="62"/>
       <c r="E4" s="62"/>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="5" spans="3:7" ht="15">
       <c r="C5" s="63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="62"/>
       <c r="E5" s="62"/>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="6" spans="3:7" ht="15">
       <c r="C6" s="63" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="62"/>
       <c r="E6" s="62"/>
@@ -1959,7 +1959,7 @@
     </row>
     <row r="7" spans="3:7" ht="15">
       <c r="C7" s="63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -1974,563 +1974,563 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="3:7" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="47" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="40"/>
+    </row>
+    <row r="10" spans="3:7" ht="15">
+      <c r="C10" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="48"/>
-    </row>
-    <row r="10" spans="3:7" ht="15">
-      <c r="C10" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="15.75" thickBot="1">
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" ht="15.75" thickBot="1">
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52" t="s">
+      <c r="G11" s="43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7">
+      <c r="C12" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="51" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7">
-      <c r="C12" s="45" t="s">
+      <c r="D12" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="E12" s="19"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="19"/>
+    </row>
+    <row r="13" spans="3:7">
+      <c r="C13" s="37"/>
+      <c r="D13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="27"/>
-    </row>
-    <row r="13" spans="3:7">
-      <c r="C13" s="45"/>
-      <c r="D13" s="27" t="s">
+      <c r="E13" s="19"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="19"/>
+    </row>
+    <row r="14" spans="3:7">
+      <c r="C14" s="37"/>
+      <c r="D14" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="3:7">
+      <c r="C15" s="37"/>
+      <c r="D15" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="19"/>
+    </row>
+    <row r="16" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C16" s="37"/>
+      <c r="D16" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="19"/>
+    </row>
+    <row r="17" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C17" s="37"/>
+      <c r="D17" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="27"/>
-    </row>
-    <row r="14" spans="3:7">
-      <c r="C14" s="45"/>
-      <c r="D14" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="27"/>
-    </row>
-    <row r="15" spans="3:7">
-      <c r="C15" s="45"/>
-      <c r="D15" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="27"/>
-    </row>
-    <row r="16" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C16" s="45"/>
-      <c r="D16" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="27"/>
-    </row>
-    <row r="17" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C17" s="45"/>
-      <c r="D17" s="42" t="s">
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="28"/>
-    </row>
-    <row r="18" spans="3:7">
-      <c r="C18" s="45" t="s">
+      <c r="D18" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="E18" s="19"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19" s="37"/>
+      <c r="D19" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="27"/>
-    </row>
-    <row r="19" spans="3:7">
-      <c r="C19" s="45"/>
-      <c r="D19" s="27" t="s">
+      <c r="E19" s="19"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="19"/>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20" s="37"/>
+      <c r="D20" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="27"/>
-    </row>
-    <row r="20" spans="3:7">
-      <c r="C20" s="45"/>
-      <c r="D20" s="27" t="s">
+      <c r="E20" s="19"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21" s="37"/>
+      <c r="D21" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="19"/>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22" s="37"/>
+      <c r="D22" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="19"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="19"/>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="C23" s="37"/>
+      <c r="D23" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="19"/>
+    </row>
+    <row r="24" spans="3:7">
+      <c r="C24" s="37"/>
+      <c r="D24" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="19"/>
+    </row>
+    <row r="25" spans="3:7">
+      <c r="C25" s="37"/>
+      <c r="D25" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="27"/>
-    </row>
-    <row r="21" spans="3:7">
-      <c r="C21" s="45"/>
-      <c r="D21" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="27"/>
-    </row>
-    <row r="22" spans="3:7">
-      <c r="C22" s="45"/>
-      <c r="D22" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="27"/>
-    </row>
-    <row r="23" spans="3:7">
-      <c r="C23" s="45"/>
-      <c r="D23" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="27"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="3:7">
-      <c r="C24" s="45"/>
-      <c r="D24" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="27"/>
-    </row>
-    <row r="25" spans="3:7">
-      <c r="C25" s="45"/>
-      <c r="D25" s="27" t="s">
+      <c r="E25" s="19"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="19"/>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="C26" s="37"/>
+      <c r="D26" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="19"/>
+    </row>
+    <row r="27" spans="3:7">
+      <c r="C27" s="37"/>
+      <c r="D27" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="19"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="19"/>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="C28" s="37"/>
+      <c r="D28" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="19"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="19"/>
+    </row>
+    <row r="29" spans="3:7">
+      <c r="C29" s="37"/>
+      <c r="D29" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="19"/>
+    </row>
+    <row r="30" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C30" s="37"/>
+      <c r="D30" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="19"/>
+    </row>
+    <row r="31" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C31" s="37"/>
+      <c r="D31" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="27"/>
-    </row>
-    <row r="26" spans="3:7">
-      <c r="C26" s="45"/>
-      <c r="D26" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="27"/>
-    </row>
-    <row r="27" spans="3:7">
-      <c r="C27" s="45"/>
-      <c r="D27" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="27"/>
-    </row>
-    <row r="28" spans="3:7">
-      <c r="C28" s="45"/>
-      <c r="D28" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="27"/>
-    </row>
-    <row r="29" spans="3:7">
-      <c r="C29" s="45"/>
-      <c r="D29" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="27"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="27"/>
-    </row>
-    <row r="30" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C30" s="45"/>
-      <c r="D30" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="27"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="27"/>
-    </row>
-    <row r="31" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C31" s="45"/>
-      <c r="D31" s="42" t="s">
+      <c r="E31" s="20"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32" spans="3:7">
+      <c r="C32" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="28"/>
-    </row>
-    <row r="32" spans="3:7">
-      <c r="C32" s="45" t="s">
+      <c r="D32" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="41" t="s">
+      <c r="E32" s="19"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33" s="37"/>
+      <c r="D33" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="27"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="27"/>
-    </row>
-    <row r="33" spans="3:7">
-      <c r="C33" s="45"/>
-      <c r="D33" s="27" t="s">
+      <c r="E33" s="19"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C34" s="37"/>
+      <c r="D34" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="27"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="27"/>
-    </row>
-    <row r="34" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C34" s="45"/>
-      <c r="D34" s="27" t="s">
+      <c r="E34" s="19"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="19"/>
+    </row>
+    <row r="35" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C35" s="37"/>
+      <c r="D35" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="27"/>
-    </row>
-    <row r="35" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C35" s="45"/>
-      <c r="D35" s="42" t="s">
+      <c r="E35" s="20"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="20"/>
+    </row>
+    <row r="36" spans="3:7">
+      <c r="C36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="28"/>
-    </row>
-    <row r="36" spans="3:7">
-      <c r="C36" s="45" t="s">
+      <c r="D36" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="41" t="s">
+      <c r="E36" s="19"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="19"/>
+    </row>
+    <row r="37" spans="3:7">
+      <c r="C37" s="37"/>
+      <c r="D37" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="27"/>
-    </row>
-    <row r="37" spans="3:7">
-      <c r="C37" s="45"/>
-      <c r="D37" s="27" t="s">
+      <c r="E37" s="19"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="19"/>
+    </row>
+    <row r="38" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C38" s="37"/>
+      <c r="D38" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="27"/>
-    </row>
-    <row r="38" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C38" s="45"/>
-      <c r="D38" s="27" t="s">
+      <c r="E38" s="19"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="19"/>
+    </row>
+    <row r="39" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C39" s="37"/>
+      <c r="D39" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="27"/>
-    </row>
-    <row r="39" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C39" s="45"/>
-      <c r="D39" s="42" t="s">
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="20"/>
+    </row>
+    <row r="40" spans="3:7">
+      <c r="C40" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="28"/>
-    </row>
-    <row r="40" spans="3:7">
-      <c r="C40" s="45" t="s">
+      <c r="D40" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="41" t="s">
+      <c r="E40" s="19"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="19"/>
+    </row>
+    <row r="41" spans="3:7">
+      <c r="C41" s="37"/>
+      <c r="D41" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="27"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="3:7">
-      <c r="C41" s="45"/>
-      <c r="D41" s="27" t="s">
+      <c r="E41" s="19"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="19"/>
+    </row>
+    <row r="42" spans="3:7">
+      <c r="C42" s="37"/>
+      <c r="D42" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="19"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="19"/>
+    </row>
+    <row r="43" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C43" s="37"/>
+      <c r="D43" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="19"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="19"/>
+    </row>
+    <row r="44" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C44" s="37"/>
+      <c r="D44" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E41" s="27"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="27"/>
-    </row>
-    <row r="42" spans="3:7">
-      <c r="C42" s="45"/>
-      <c r="D42" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E42" s="27"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="27"/>
-    </row>
-    <row r="43" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C43" s="45"/>
-      <c r="D43" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="27"/>
-    </row>
-    <row r="44" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C44" s="45"/>
-      <c r="D44" s="42" t="s">
+      <c r="E44" s="20"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="20"/>
+    </row>
+    <row r="45" spans="3:7">
+      <c r="C45" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="E44" s="28"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="28"/>
-    </row>
-    <row r="45" spans="3:7">
-      <c r="C45" s="45" t="s">
+      <c r="D45" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="41" t="s">
+      <c r="E45" s="19"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="19"/>
+    </row>
+    <row r="46" spans="3:7">
+      <c r="C46" s="37"/>
+      <c r="D46" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="19"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="19"/>
+    </row>
+    <row r="47" spans="3:7">
+      <c r="C47" s="37"/>
+      <c r="D47" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E47" s="19"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="19"/>
+    </row>
+    <row r="48" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C48" s="37"/>
+      <c r="D48" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E48" s="19"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="19"/>
+    </row>
+    <row r="49" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C49" s="37"/>
+      <c r="D49" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="27"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="27"/>
-    </row>
-    <row r="46" spans="3:7">
-      <c r="C46" s="45"/>
-      <c r="D46" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E46" s="27"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="27"/>
-    </row>
-    <row r="47" spans="3:7">
-      <c r="C47" s="45"/>
-      <c r="D47" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" s="27"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="27"/>
-    </row>
-    <row r="48" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C48" s="45"/>
-      <c r="D48" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E48" s="27"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="27"/>
-    </row>
-    <row r="49" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C49" s="45"/>
-      <c r="D49" s="42" t="s">
+      <c r="E49" s="20"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="20"/>
+    </row>
+    <row r="50" spans="3:7">
+      <c r="C50" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="E49" s="28"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="28"/>
-    </row>
-    <row r="50" spans="3:7">
-      <c r="C50" s="45" t="s">
+      <c r="D50" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="41" t="s">
+      <c r="E50" s="19"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="19"/>
+    </row>
+    <row r="51" spans="3:7">
+      <c r="C51" s="37"/>
+      <c r="D51" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E50" s="27"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="27"/>
-    </row>
-    <row r="51" spans="3:7">
-      <c r="C51" s="45"/>
-      <c r="D51" s="27" t="s">
+      <c r="E51" s="19"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="19"/>
+    </row>
+    <row r="52" spans="3:7">
+      <c r="C52" s="37"/>
+      <c r="D52" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="27"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="27"/>
-    </row>
-    <row r="52" spans="3:7">
-      <c r="C52" s="45"/>
-      <c r="D52" s="27" t="s">
+      <c r="E52" s="19"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="19"/>
+    </row>
+    <row r="53" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C53" s="37"/>
+      <c r="D53" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E52" s="27"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="27"/>
-    </row>
-    <row r="53" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C53" s="45"/>
-      <c r="D53" s="27" t="s">
+      <c r="E53" s="19"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="19"/>
+    </row>
+    <row r="54" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C54" s="37"/>
+      <c r="D54" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="E53" s="27"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="27"/>
-    </row>
-    <row r="54" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C54" s="45"/>
-      <c r="D54" s="42" t="s">
+      <c r="E54" s="20"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="20"/>
+    </row>
+    <row r="55" spans="3:7">
+      <c r="C55" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="E54" s="28"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="28"/>
-    </row>
-    <row r="55" spans="3:7">
-      <c r="C55" s="45" t="s">
+      <c r="D55" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="D55" s="41" t="s">
+      <c r="E55" s="19"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="19"/>
+    </row>
+    <row r="56" spans="3:7">
+      <c r="C56" s="18"/>
+      <c r="D56" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E56" s="19"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="19"/>
+    </row>
+    <row r="57" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C57" s="18"/>
+      <c r="D57" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E57" s="19"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="19"/>
+    </row>
+    <row r="58" spans="3:7" ht="13.5" thickBot="1">
+      <c r="C58" s="18"/>
+      <c r="D58" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="E55" s="27"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="27"/>
-    </row>
-    <row r="56" spans="3:7">
-      <c r="C56" s="26"/>
-      <c r="D56" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E56" s="27"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="27"/>
-    </row>
-    <row r="57" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C57" s="26"/>
-      <c r="D57" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E57" s="27"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="27"/>
-    </row>
-    <row r="58" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C58" s="26"/>
-      <c r="D58" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="E58" s="28"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="28"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="20"/>
     </row>
     <row r="59" spans="3:7">
-      <c r="C59" s="30"/>
-      <c r="D59" s="31"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="23"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
-      <c r="G59" s="27"/>
+      <c r="G59" s="19"/>
     </row>
     <row r="60" spans="3:7">
-      <c r="C60" s="30"/>
-      <c r="D60" s="31"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="23"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
-      <c r="G60" s="27"/>
+      <c r="G60" s="19"/>
     </row>
     <row r="61" spans="3:7">
-      <c r="C61" s="30"/>
-      <c r="D61" s="31"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="23"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
-      <c r="G61" s="27"/>
+      <c r="G61" s="19"/>
     </row>
     <row r="62" spans="3:7">
-      <c r="C62" s="30"/>
-      <c r="D62" s="31"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="23"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
-      <c r="G62" s="27"/>
+      <c r="G62" s="19"/>
     </row>
     <row r="63" spans="3:7" ht="13.5" thickBot="1">
-      <c r="C63" s="32"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="35"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="27"/>
     </row>
     <row r="64" spans="3:7">
-      <c r="C64" s="43" t="s">
-        <v>68</v>
+      <c r="C64" s="35" t="s">
+        <v>67</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="27"/>
+      <c r="G64" s="19"/>
     </row>
     <row r="65" spans="1:7" ht="13.5" thickBot="1">
-      <c r="C65" s="44" t="s">
+      <c r="C65" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="27"/>
+    </row>
+    <row r="66" spans="1:7" ht="13.5" thickBot="1">
+      <c r="C66" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="35"/>
-    </row>
-    <row r="66" spans="1:7" ht="13.5" thickBot="1">
-      <c r="C66" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="38"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="30"/>
     </row>
     <row r="67" spans="1:7" ht="13.5" thickTop="1">
-      <c r="C67" s="39"/>
+      <c r="C67" s="31"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
     </row>
     <row r="68" spans="1:7" ht="14.25">
-      <c r="A68" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="C68" s="40"/>
+      <c r="A68" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="32"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
     </row>
     <row r="69" spans="1:7" ht="14.25">
-      <c r="A69" s="53"/>
-      <c r="C69" s="40"/>
+      <c r="A69" s="45"/>
+      <c r="C69" s="32"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>

</xml_diff>

<commit_message>
beresin lampiran rks penunjukan langsung
</commit_message>
<xml_diff>
--- a/templates/PL-B-Lamp_2.xlsx
+++ b/templates/PL-B-Lamp_2.xlsx
@@ -1068,9 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:H6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -1901,7 +1899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView topLeftCell="B49" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6:G6"/>
     </sheetView>
   </sheetViews>

</xml_diff>